<commit_message>
feat: update docs and templates to fit datamodel changes
</commit_message>
<xml_diff>
--- a/docs/resources/Dictionary.xlsx
+++ b/docs/resources/Dictionary.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\brend\projects\catalogue\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\brend\Molgenis\repos\molgenis-emx2\docs\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5C487E0B-7075-44C5-B210-ECBD0BBB8894}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F158DA4-A40B-4737-AAB6-41EB8048B14F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="800" yWindow="600" windowWidth="18400" windowHeight="10200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3880" yWindow="2920" windowWidth="10440" windowHeight="7880" firstSheet="4" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SourceTables" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="21">
   <si>
     <t>name</t>
   </si>
@@ -83,12 +83,6 @@
     <t>isRepeatOf.name</t>
   </si>
   <si>
-    <t>ageMin</t>
-  </si>
-  <si>
-    <t>ageMax</t>
-  </si>
-  <si>
     <t>subcohorts</t>
   </si>
   <si>
@@ -96,6 +90,9 @@
   </si>
   <si>
     <t>numberOfRows</t>
+  </si>
+  <si>
+    <t>ageGroups</t>
   </si>
 </sst>
 </file>
@@ -361,7 +358,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
@@ -386,10 +383,10 @@
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -4580,23 +4577,23 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:E1000"/>
+  <dimension ref="A1:D1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:E1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="7.6640625" customWidth="1"/>
     <col min="2" max="2" width="18" customWidth="1"/>
-    <col min="3" max="4" width="7.6640625" customWidth="1"/>
-    <col min="5" max="5" width="9.4140625" customWidth="1"/>
-    <col min="6" max="6" width="20.6640625" customWidth="1"/>
-    <col min="7" max="26" width="7.6640625" customWidth="1"/>
+    <col min="3" max="3" width="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.4140625" customWidth="1"/>
+    <col min="5" max="5" width="20.6640625" customWidth="1"/>
+    <col min="6" max="25" width="7.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4604,30 +4601,27 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>19</v>
-      </c>
     </row>
-    <row r="2" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="4" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="5" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="6" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="7" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="8" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="9" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="10" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="11" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="12" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="13" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="14" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="15" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="16" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="4" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="5" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="6" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="7" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="8" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="9" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="10" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="11" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="12" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="13" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="14" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="15" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="16" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="17" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="18" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
feat: update templates and docs to fit new data model
</commit_message>
<xml_diff>
--- a/docs/resources/Dictionary.xlsx
+++ b/docs/resources/Dictionary.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\brend\projects\catalogue\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\brend\Molgenis\repos\molgenis-emx2\docs\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5C487E0B-7075-44C5-B210-ECBD0BBB8894}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36F38C70-1467-43BA-A507-6B8EF6109D7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="800" yWindow="600" windowWidth="18400" windowHeight="10200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3880" yWindow="2920" windowWidth="10440" windowHeight="7880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SourceTables" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="21">
   <si>
     <t>name</t>
   </si>
@@ -83,12 +83,6 @@
     <t>isRepeatOf.name</t>
   </si>
   <si>
-    <t>ageMin</t>
-  </si>
-  <si>
-    <t>ageMax</t>
-  </si>
-  <si>
     <t>subcohorts</t>
   </si>
   <si>
@@ -96,6 +90,9 @@
   </si>
   <si>
     <t>numberOfRows</t>
+  </si>
+  <si>
+    <t>ageGroups</t>
   </si>
 </sst>
 </file>
@@ -386,10 +383,10 @@
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -4580,23 +4577,23 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:E1000"/>
+  <dimension ref="A1:D1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:E1"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="7.6640625" customWidth="1"/>
     <col min="2" max="2" width="18" customWidth="1"/>
-    <col min="3" max="4" width="7.6640625" customWidth="1"/>
-    <col min="5" max="5" width="9.4140625" customWidth="1"/>
-    <col min="6" max="6" width="20.6640625" customWidth="1"/>
-    <col min="7" max="26" width="7.6640625" customWidth="1"/>
+    <col min="3" max="3" width="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.4140625" customWidth="1"/>
+    <col min="5" max="5" width="20.6640625" customWidth="1"/>
+    <col min="6" max="25" width="7.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4604,30 +4601,27 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>19</v>
-      </c>
     </row>
-    <row r="2" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="4" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="5" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="6" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="7" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="8" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="9" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="10" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="11" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="12" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="13" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="14" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="15" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="16" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="4" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="5" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="6" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="7" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="8" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="9" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="10" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="11" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="12" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="13" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="14" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="15" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="16" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="17" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="18" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
fix templates for dictionary uploads
</commit_message>
<xml_diff>
--- a/docs/resources/Dictionary.xlsx
+++ b/docs/resources/Dictionary.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\brend\Molgenis\repos\molgenis-emx2\docs\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{150D292C-33B4-4EFB-923C-D786B1585E78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CB5D145-FCA1-4EB1-A4D5-355F1EC7BF44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19395" windowHeight="12195" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15" yWindow="15" windowWidth="19185" windowHeight="11985" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Datasets" sheetId="9" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="28">
   <si>
     <t>label</t>
   </si>
@@ -103,6 +103,9 @@
   </si>
   <si>
     <t>useExternalDefinition.name</t>
+  </si>
+  <si>
+    <t>variable</t>
   </si>
 </sst>
 </file>
@@ -633,13 +636,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
   <dimension ref="A1:J1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="7.59765625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="6.59765625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.1328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.86328125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="4.86328125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="4.53125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="4.86328125" bestFit="1" customWidth="1"/>
@@ -657,7 +662,7 @@
         <v>14</v>
       </c>
       <c r="C1" t="s">
-        <v>3</v>
+        <v>27</v>
       </c>
       <c r="D1" t="s">
         <v>11</v>

</xml_diff>

<commit_message>
fix templates for dictionary uploads (#4940)
</commit_message>
<xml_diff>
--- a/docs/resources/Dictionary.xlsx
+++ b/docs/resources/Dictionary.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\brend\Molgenis\repos\molgenis-emx2\docs\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{150D292C-33B4-4EFB-923C-D786B1585E78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CB5D145-FCA1-4EB1-A4D5-355F1EC7BF44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19395" windowHeight="12195" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15" yWindow="15" windowWidth="19185" windowHeight="11985" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Datasets" sheetId="9" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="28">
   <si>
     <t>label</t>
   </si>
@@ -103,6 +103,9 @@
   </si>
   <si>
     <t>useExternalDefinition.name</t>
+  </si>
+  <si>
+    <t>variable</t>
   </si>
 </sst>
 </file>
@@ -633,13 +636,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
   <dimension ref="A1:J1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="7.59765625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="6.59765625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.1328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.86328125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="4.86328125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="4.53125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="4.86328125" bestFit="1" customWidth="1"/>
@@ -657,7 +662,7 @@
         <v>14</v>
       </c>
       <c r="C1" t="s">
-        <v>3</v>
+        <v>27</v>
       </c>
       <c r="D1" t="s">
         <v>11</v>

</xml_diff>